<commit_message>
Updated website articles and added a privacy notification on the calculation page
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF2E56C-559B-4CFD-86E8-05A78D495FFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEACAA6-34F3-4240-B070-D7A07C4539E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
+    <workbookView xWindow="3750" yWindow="1860" windowWidth="20910" windowHeight="11835" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Order</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>Paycheck replacement coverage is scarce, if it exists at all. …</t>
+  </si>
+  <si>
+    <t>https://www.sapling.com/11368489/can-collect-unemployment-after-graduation-graduate-school</t>
+  </si>
+  <si>
+    <t>Even if you applied yourself diligently throughout your final year in grad school seeking a job to kick off your career …</t>
+  </si>
+  <si>
+    <t>Can I Collect Unemployment After Graduation From Graduate School?</t>
+  </si>
+  <si>
+    <t>https://bizfluent.com/info-10060450-can-college-students-receive-unemployment-benefits.html</t>
+  </si>
+  <si>
+    <t>Can College Students Receive Unemployment Benefits?</t>
+  </si>
+  <si>
+    <t>The traditional image of the unemployed doesn’t usually include college students. However, many college students …</t>
   </si>
 </sst>
 </file>
@@ -600,13 +618,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012018ED-ADEC-411C-8179-D619E26FC50D}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,16 +676,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="9">
-        <v>43420</v>
+        <v>43004</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -675,16 +693,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="9">
-        <v>43524</v>
+        <v>43420</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -692,16 +710,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="9">
-        <v>42991</v>
+        <v>43524</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -709,16 +727,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="9">
-        <v>43525</v>
+        <v>42991</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -726,16 +744,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="9">
-        <v>42677</v>
+        <v>43525</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -743,16 +761,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="9">
-        <v>42590</v>
+        <v>42677</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -760,16 +778,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="9">
-        <v>43521</v>
+        <v>42590</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,16 +795,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="9">
-        <v>42538</v>
+        <v>43521</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -794,16 +812,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="9">
-        <v>43520</v>
+        <v>42538</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -811,16 +829,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="9">
-        <v>42518</v>
+        <v>43520</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -828,16 +846,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="9">
-        <v>41334</v>
+        <v>40773</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,16 +863,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="9">
-        <v>43523</v>
+        <v>42518</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -862,36 +880,77 @@
         <v>14</v>
       </c>
       <c r="C16" s="9">
+        <v>41334</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9">
+        <v>43523</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="9">
         <v>40033</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:F18" xr:uid="{275430C7-76EB-46D1-AB8F-7BB07CBE6685}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F18">
+      <sortCondition ref="B2:B18"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{0D8F78F3-4D89-41A9-8232-516FBE7F8FFD}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{AAEEB838-A718-4068-A64D-B0DE94FF6966}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{970420A8-ADA4-42C9-8107-6F5896533455}"/>
-    <hyperlink ref="D10" r:id="rId4" xr:uid="{A976ABDD-14CE-4B22-866B-5BCCFFECEC1F}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{510B5788-10F1-4179-ABB9-0729400F874D}"/>
-    <hyperlink ref="D15" r:id="rId6" xr:uid="{4B837B75-B744-422C-B387-36B6B0701072}"/>
-    <hyperlink ref="D4" r:id="rId7" xr:uid="{64F542A9-F445-4248-89C6-D9D649F106ED}"/>
-    <hyperlink ref="D6" r:id="rId8" xr:uid="{9BAD332B-731C-499E-BA71-C6A48F5F3D38}"/>
-    <hyperlink ref="D8" r:id="rId9" xr:uid="{B1E99C61-F53F-4474-923D-70F5429BF1D0}"/>
-    <hyperlink ref="D9" r:id="rId10" xr:uid="{B56B01DC-AACA-4BFF-9375-04138997F6A2}"/>
-    <hyperlink ref="D11" r:id="rId11" xr:uid="{9D00AA3F-2907-43CD-B0F9-8D25A1DACC02}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{1110A2D7-4E13-4260-B304-EC10DAF84D40}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{22C079E4-6DC0-48DB-B09C-A092E01FB12D}"/>
-    <hyperlink ref="D16" r:id="rId14" xr:uid="{1EA15340-F74B-4FAE-A861-A2DFF13A57A6}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{AAEEB838-A718-4068-A64D-B0DE94FF6966}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{970420A8-ADA4-42C9-8107-6F5896533455}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{A976ABDD-14CE-4B22-866B-5BCCFFECEC1F}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{510B5788-10F1-4179-ABB9-0729400F874D}"/>
+    <hyperlink ref="D17" r:id="rId6" xr:uid="{4B837B75-B744-422C-B387-36B6B0701072}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{64F542A9-F445-4248-89C6-D9D649F106ED}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{9BAD332B-731C-499E-BA71-C6A48F5F3D38}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{B1E99C61-F53F-4474-923D-70F5429BF1D0}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{B56B01DC-AACA-4BFF-9375-04138997F6A2}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{9D00AA3F-2907-43CD-B0F9-8D25A1DACC02}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{1110A2D7-4E13-4260-B304-EC10DAF84D40}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{22C079E4-6DC0-48DB-B09C-A092E01FB12D}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{1EA15340-F74B-4FAE-A861-A2DFF13A57A6}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{719F5CCC-B404-4243-B545-073E07F78C68}"/>
+    <hyperlink ref="D4" r:id="rId16" xr:uid="{FFDF4DD0-6A5B-4ED2-9F8E-D381723AC418}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switching away from the "Months of Coverage" presentation, added some new articles, and changed the database name
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEACAA6-34F3-4240-B070-D7A07C4539E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF43F16-F32E-4376-8D7B-EBE98E0AC792}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="1860" windowWidth="20910" windowHeight="11835" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$F$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Order</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>The traditional image of the unemployed doesn’t usually include college students. However, many college students …</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2019/05/11/opinion/sunday/student-loans.html</t>
+  </si>
+  <si>
+    <t>As American families refresh the wait lists and weigh their aid offers, yet another cohort of children sets foot into our disaster …</t>
+  </si>
+  <si>
+    <t>What’s Scarier Than Student Loans? Welcome to the World of Subprime Children</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/news/articles/2019-05-12/u-s-stepping-up-enforcement-on-delinquent-student-loans</t>
+  </si>
+  <si>
+    <t>U.S. Stepping Up Enforcement on Delinquent Student Loans</t>
+  </si>
+  <si>
+    <t>The U.S. government stepped up collections on delinquent student debt to $2.9 billion last year ...</t>
   </si>
 </sst>
 </file>
@@ -232,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -271,12 +289,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -297,11 +324,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -618,13 +654,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012018ED-ADEC-411C-8179-D619E26FC50D}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,298 +695,334 @@
         <v>1</v>
       </c>
       <c r="C3" s="7">
+        <v>43596</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10">
         <v>43522</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9">
+    <row r="5" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10">
         <v>43004</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+    <row r="6" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43597</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43420</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8">
+        <v>43524</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8">
+        <v>42991</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
+        <v>43525</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8">
+        <v>42677</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8">
+        <v>42590</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8">
+        <v>43521</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8">
+        <v>42538</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8">
+        <v>43520</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8">
+        <v>40773</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8">
+        <v>42518</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
+        <v>16</v>
+      </c>
+      <c r="C18" s="8">
+        <v>41334</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9">
+        <v>17</v>
+      </c>
+      <c r="C19" s="8">
+        <v>43523</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9">
+        <v>18</v>
+      </c>
+      <c r="C20" s="8">
+        <v>40033</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9">
-        <v>43420</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9">
-        <v>43524</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9">
-        <v>42991</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="9">
-        <v>43525</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9">
-        <v>42677</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
-        <v>8</v>
-      </c>
-      <c r="C10" s="9">
-        <v>42590</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
-        <v>9</v>
-      </c>
-      <c r="C11" s="9">
-        <v>43521</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9">
-        <v>42538</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
-        <v>11</v>
-      </c>
-      <c r="C13" s="9">
-        <v>43520</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
-        <v>12</v>
-      </c>
-      <c r="C14" s="9">
-        <v>40773</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
-        <v>13</v>
-      </c>
-      <c r="C15" s="9">
-        <v>42518</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
-        <v>14</v>
-      </c>
-      <c r="C16" s="9">
-        <v>41334</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
-        <v>15</v>
-      </c>
-      <c r="C17" s="9">
-        <v>43523</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
-        <v>16</v>
-      </c>
-      <c r="C18" s="9">
-        <v>40033</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F18" xr:uid="{275430C7-76EB-46D1-AB8F-7BB07CBE6685}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F18">
-      <sortCondition ref="B2:B18"/>
+  <autoFilter ref="B2:F20" xr:uid="{275430C7-76EB-46D1-AB8F-7BB07CBE6685}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F20">
+      <sortCondition ref="B2:B20"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{0D8F78F3-4D89-41A9-8232-516FBE7F8FFD}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{AAEEB838-A718-4068-A64D-B0DE94FF6966}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{970420A8-ADA4-42C9-8107-6F5896533455}"/>
-    <hyperlink ref="D11" r:id="rId4" xr:uid="{A976ABDD-14CE-4B22-866B-5BCCFFECEC1F}"/>
-    <hyperlink ref="D13" r:id="rId5" xr:uid="{510B5788-10F1-4179-ABB9-0729400F874D}"/>
-    <hyperlink ref="D17" r:id="rId6" xr:uid="{4B837B75-B744-422C-B387-36B6B0701072}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{64F542A9-F445-4248-89C6-D9D649F106ED}"/>
-    <hyperlink ref="D7" r:id="rId8" xr:uid="{9BAD332B-731C-499E-BA71-C6A48F5F3D38}"/>
-    <hyperlink ref="D9" r:id="rId9" xr:uid="{B1E99C61-F53F-4474-923D-70F5429BF1D0}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{B56B01DC-AACA-4BFF-9375-04138997F6A2}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{9D00AA3F-2907-43CD-B0F9-8D25A1DACC02}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{1110A2D7-4E13-4260-B304-EC10DAF84D40}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{22C079E4-6DC0-48DB-B09C-A092E01FB12D}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{1EA15340-F74B-4FAE-A861-A2DFF13A57A6}"/>
-    <hyperlink ref="D14" r:id="rId15" xr:uid="{719F5CCC-B404-4243-B545-073E07F78C68}"/>
-    <hyperlink ref="D4" r:id="rId16" xr:uid="{FFDF4DD0-6A5B-4ED2-9F8E-D381723AC418}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{0D8F78F3-4D89-41A9-8232-516FBE7F8FFD}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{AAEEB838-A718-4068-A64D-B0DE94FF6966}"/>
+    <hyperlink ref="D10" r:id="rId3" xr:uid="{970420A8-ADA4-42C9-8107-6F5896533455}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{A976ABDD-14CE-4B22-866B-5BCCFFECEC1F}"/>
+    <hyperlink ref="D15" r:id="rId5" xr:uid="{510B5788-10F1-4179-ABB9-0729400F874D}"/>
+    <hyperlink ref="D19" r:id="rId6" xr:uid="{4B837B75-B744-422C-B387-36B6B0701072}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{64F542A9-F445-4248-89C6-D9D649F106ED}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{9BAD332B-731C-499E-BA71-C6A48F5F3D38}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{B1E99C61-F53F-4474-923D-70F5429BF1D0}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{B56B01DC-AACA-4BFF-9375-04138997F6A2}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{9D00AA3F-2907-43CD-B0F9-8D25A1DACC02}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{1110A2D7-4E13-4260-B304-EC10DAF84D40}"/>
+    <hyperlink ref="D18" r:id="rId13" xr:uid="{22C079E4-6DC0-48DB-B09C-A092E01FB12D}"/>
+    <hyperlink ref="D20" r:id="rId14" xr:uid="{1EA15340-F74B-4FAE-A861-A2DFF13A57A6}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{719F5CCC-B404-4243-B545-073E07F78C68}"/>
+    <hyperlink ref="D5" r:id="rId16" xr:uid="{FFDF4DD0-6A5B-4ED2-9F8E-D381723AC418}"/>
+    <hyperlink ref="D3" r:id="rId17" xr:uid="{F75543D1-BB27-4DDA-AD76-4CF162DE5BC4}"/>
+    <hyperlink ref="D6" r:id="rId18" xr:uid="{E12414E5-71D7-411D-9D91-9E66631179DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor debugging of a problem with the email formatting of results
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF43F16-F32E-4376-8D7B-EBE98E0AC792}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139BB1AD-5438-47C2-89D1-15A05F3D62E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
   </bookViews>
@@ -660,7 +660,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EDSF-72: Last bit of fine tuning to get the instituations home page up and running
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-Posted-Articles.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139BB1AD-5438-47C2-89D1-15A05F3D62E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0D50EE-8ED0-43CD-953F-23FE37CE947A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
+    <workbookView xWindow="1710" yWindow="90" windowWidth="17535" windowHeight="11430" xr2:uid="{7266D3BB-B4C0-4D55-8728-C93F95E2A2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$F$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$B$2:$F$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Order</t>
   </si>
@@ -211,6 +211,60 @@
   </si>
   <si>
     <t>The U.S. government stepped up collections on delinquent student debt to $2.9 billion last year ...</t>
+  </si>
+  <si>
+    <t>https://www.cbsnews.com/news/student-loan-debt-bipartisan-proposal-would-help-employers-ease-debt/</t>
+  </si>
+  <si>
+    <t>Bill to Help Employers Ease Student Loan Debt Backed by Both Parties</t>
+  </si>
+  <si>
+    <t>https://www.unemployment-tips.com/can-i-collect-unemployment-after-graduating-grad-school-and-not-finding-a-job.html</t>
+  </si>
+  <si>
+    <t>Can I Collect Unemployment After Graduating Grad School and Not Finding a Job?</t>
+  </si>
+  <si>
+    <t>I am interested in finding out if I can apply for unemployment since I just graduated from Graduate School …</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2019/06/25/upshot/student-loan-debt-forgiveness.html</t>
+  </si>
+  <si>
+    <t>Canceling Student Loan Debt Doesn’t Make Problems Disappear</t>
+  </si>
+  <si>
+    <t>Senator Bernie Sanders proposed canceling all outstanding student loan debt in the United States …</t>
+  </si>
+  <si>
+    <t>A proposed tax incentive for businesses could bring relief for Americans saddled with student debt …</t>
+  </si>
+  <si>
+    <t>https://www.insidehighered.com/views/2019/06/18/congress-should-obligate-colleges-help-repay-students-debt-opinion</t>
+  </si>
+  <si>
+    <t>Colleges Should Cosign Student Loans</t>
+  </si>
+  <si>
+    <t>More than 16 million students are enrolled in the nation’s higher education institutions today. But only about 60 percent …</t>
+  </si>
+  <si>
+    <t>https://finance.yahoo.com/news/jpmorgan-ceo-jamie-dimon-calls-student-loans-a-disgrace-171749043.html</t>
+  </si>
+  <si>
+    <t>JPMorgan's Jamie Dimon: Student Lending in the U.S. is a 'Disgrace' and It's 'Hurting America'</t>
+  </si>
+  <si>
+    <t>JPMorgan Chase (JPM) CEO Jamie Dimon says student lending in the U.S. has been 'a disgrace' and it's 'hurting America.' …</t>
+  </si>
+  <si>
+    <t>https://www.npr.org/2019/07/09/738985632/these-are-the-people-struggling-the-most-to-pay-back-student-loans</t>
+  </si>
+  <si>
+    <t>These Are The People Struggling The Most To Pay Back Student Loans</t>
+  </si>
+  <si>
+    <t>Lots of people have student loans: more than 45 million people. They collectively owe about $1.6 trillion …</t>
   </si>
 </sst>
 </file>
@@ -654,13 +708,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012018ED-ADEC-411C-8179-D619E26FC50D}">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,16 +749,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="7">
-        <v>43596</v>
+        <v>43655</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -712,16 +766,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="10">
-        <v>43522</v>
+        <v>43641</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,84 +783,84 @@
         <v>3</v>
       </c>
       <c r="C5" s="10">
-        <v>43004</v>
+        <v>43525</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
-        <v>43597</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>58</v>
+      <c r="C6" s="10">
+        <v>43641</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="8">
-        <v>43420</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>39</v>
+      <c r="C7" s="10">
+        <v>43634</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="8">
-        <v>43524</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
+      <c r="C8" s="10">
+        <v>43609</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" s="8">
-        <v>42991</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
+      <c r="C9" s="10">
+        <v>43597</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -814,33 +868,33 @@
         <v>8</v>
       </c>
       <c r="C10" s="8">
-        <v>43525</v>
+        <v>43522</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="8">
-        <v>42677</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>41</v>
+      <c r="C11" s="10">
+        <v>43596</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -848,16 +902,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="8">
-        <v>42590</v>
+        <v>43523</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,16 +919,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="8">
-        <v>43521</v>
+        <v>43520</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -882,16 +936,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="8">
-        <v>42538</v>
+        <v>43420</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -899,33 +953,33 @@
         <v>13</v>
       </c>
       <c r="C15" s="8">
-        <v>43520</v>
+        <v>43004</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>14</v>
       </c>
-      <c r="C16" s="8">
-        <v>40773</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>48</v>
+      <c r="C16" s="10">
+        <v>43524</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -933,16 +987,16 @@
         <v>15</v>
       </c>
       <c r="C17" s="8">
-        <v>42518</v>
+        <v>42991</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -950,16 +1004,16 @@
         <v>16</v>
       </c>
       <c r="C18" s="8">
-        <v>41334</v>
+        <v>42677</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,16 +1021,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="8">
-        <v>43523</v>
+        <v>42590</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -984,45 +1038,153 @@
         <v>18</v>
       </c>
       <c r="C20" s="8">
+        <v>42538</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="9">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8">
+        <v>43521</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8">
+        <v>42518</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="9">
+        <v>21</v>
+      </c>
+      <c r="C23" s="8">
+        <v>41334</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="9">
+        <v>22</v>
+      </c>
+      <c r="C24" s="8">
+        <v>40773</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="9">
+        <v>23</v>
+      </c>
+      <c r="C25" s="8">
+        <v>40377</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
+        <v>24</v>
+      </c>
+      <c r="C26" s="8">
         <v>40033</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F20" xr:uid="{275430C7-76EB-46D1-AB8F-7BB07CBE6685}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F20">
-      <sortCondition ref="B2:B20"/>
+  <autoFilter ref="B2:F26" xr:uid="{275430C7-76EB-46D1-AB8F-7BB07CBE6685}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F26">
+      <sortCondition descending="1" ref="C2:C26"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{0D8F78F3-4D89-41A9-8232-516FBE7F8FFD}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{AAEEB838-A718-4068-A64D-B0DE94FF6966}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{970420A8-ADA4-42C9-8107-6F5896533455}"/>
-    <hyperlink ref="D13" r:id="rId4" xr:uid="{A976ABDD-14CE-4B22-866B-5BCCFFECEC1F}"/>
-    <hyperlink ref="D15" r:id="rId5" xr:uid="{510B5788-10F1-4179-ABB9-0729400F874D}"/>
-    <hyperlink ref="D19" r:id="rId6" xr:uid="{4B837B75-B744-422C-B387-36B6B0701072}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{64F542A9-F445-4248-89C6-D9D649F106ED}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{9BAD332B-731C-499E-BA71-C6A48F5F3D38}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{B1E99C61-F53F-4474-923D-70F5429BF1D0}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{B56B01DC-AACA-4BFF-9375-04138997F6A2}"/>
-    <hyperlink ref="D14" r:id="rId11" xr:uid="{9D00AA3F-2907-43CD-B0F9-8D25A1DACC02}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{1110A2D7-4E13-4260-B304-EC10DAF84D40}"/>
-    <hyperlink ref="D18" r:id="rId13" xr:uid="{22C079E4-6DC0-48DB-B09C-A092E01FB12D}"/>
-    <hyperlink ref="D20" r:id="rId14" xr:uid="{1EA15340-F74B-4FAE-A861-A2DFF13A57A6}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{719F5CCC-B404-4243-B545-073E07F78C68}"/>
-    <hyperlink ref="D5" r:id="rId16" xr:uid="{FFDF4DD0-6A5B-4ED2-9F8E-D381723AC418}"/>
-    <hyperlink ref="D3" r:id="rId17" xr:uid="{F75543D1-BB27-4DDA-AD76-4CF162DE5BC4}"/>
-    <hyperlink ref="D6" r:id="rId18" xr:uid="{E12414E5-71D7-411D-9D91-9E66631179DD}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{0D8F78F3-4D89-41A9-8232-516FBE7F8FFD}"/>
+    <hyperlink ref="D16" r:id="rId2" xr:uid="{AAEEB838-A718-4068-A64D-B0DE94FF6966}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{970420A8-ADA4-42C9-8107-6F5896533455}"/>
+    <hyperlink ref="D21" r:id="rId4" xr:uid="{A976ABDD-14CE-4B22-866B-5BCCFFECEC1F}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{510B5788-10F1-4179-ABB9-0729400F874D}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{4B837B75-B744-422C-B387-36B6B0701072}"/>
+    <hyperlink ref="D14" r:id="rId7" xr:uid="{64F542A9-F445-4248-89C6-D9D649F106ED}"/>
+    <hyperlink ref="D17" r:id="rId8" xr:uid="{9BAD332B-731C-499E-BA71-C6A48F5F3D38}"/>
+    <hyperlink ref="D18" r:id="rId9" xr:uid="{B1E99C61-F53F-4474-923D-70F5429BF1D0}"/>
+    <hyperlink ref="D19" r:id="rId10" xr:uid="{B56B01DC-AACA-4BFF-9375-04138997F6A2}"/>
+    <hyperlink ref="D20" r:id="rId11" xr:uid="{9D00AA3F-2907-43CD-B0F9-8D25A1DACC02}"/>
+    <hyperlink ref="D22" r:id="rId12" xr:uid="{1110A2D7-4E13-4260-B304-EC10DAF84D40}"/>
+    <hyperlink ref="D23" r:id="rId13" xr:uid="{22C079E4-6DC0-48DB-B09C-A092E01FB12D}"/>
+    <hyperlink ref="D26" r:id="rId14" xr:uid="{1EA15340-F74B-4FAE-A861-A2DFF13A57A6}"/>
+    <hyperlink ref="D24" r:id="rId15" xr:uid="{719F5CCC-B404-4243-B545-073E07F78C68}"/>
+    <hyperlink ref="D15" r:id="rId16" xr:uid="{FFDF4DD0-6A5B-4ED2-9F8E-D381723AC418}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{F75543D1-BB27-4DDA-AD76-4CF162DE5BC4}"/>
+    <hyperlink ref="D9" r:id="rId18" xr:uid="{E12414E5-71D7-411D-9D91-9E66631179DD}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{C2355D1A-A17D-4B94-B249-692B123CB07B}"/>
+    <hyperlink ref="D25" r:id="rId20" xr:uid="{B80AB90E-6C61-48A4-9BA6-82B271C769C3}"/>
+    <hyperlink ref="D4" r:id="rId21" xr:uid="{D90FF701-1C9D-4375-B0CC-BE267B83949A}"/>
+    <hyperlink ref="D7" r:id="rId22" xr:uid="{87619550-8CD8-477B-A038-56F1327DA1A3}"/>
+    <hyperlink ref="D6" r:id="rId23" xr:uid="{FC9A1BC2-9EE0-4CF2-B987-EDA1DBA9E9EF}"/>
+    <hyperlink ref="D3" r:id="rId24" xr:uid="{F5C5B937-3555-413A-ADCF-9C14B6127A68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>